<commit_message>
Move exp to experiment folder
</commit_message>
<xml_diff>
--- a/experiment/subject_log.xlsx
+++ b/experiment/subject_log.xlsx
@@ -2,14 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\khen_heller\subliminal_priming_w_motion_capture\experiment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,26 +23,189 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="40">
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>subject num</t>
+  </si>
+  <si>
+    <t>subject age</t>
+  </si>
+  <si>
+    <t>first language</t>
+  </si>
+  <si>
+    <t>subject dom_hand</t>
+  </si>
+  <si>
+    <t>subject dom_eye</t>
+  </si>
+  <si>
+    <t>visual acuity (glasses/lenses/N)</t>
+  </si>
+  <si>
+    <t>Color Blindness (Y/N)</t>
+  </si>
+  <si>
+    <t>subject gender</t>
+  </si>
+  <si>
+    <t>Criteria? (Y/N)</t>
+  </si>
+  <si>
+    <t>payment/credit</t>
+  </si>
+  <si>
+    <t>Agrees to DB?</t>
+  </si>
+  <si>
+    <t>Agrees to be contacted again? (Y/N)</t>
+  </si>
+  <si>
+    <t>form of contact(P/E/N)</t>
+  </si>
+  <si>
+    <t>experiment version (software)</t>
+  </si>
+  <si>
+    <t>experiment room</t>
+  </si>
+  <si>
+    <t>electrode set</t>
+  </si>
+  <si>
+    <t>external set</t>
+  </si>
+  <si>
+    <t>amplifier</t>
+  </si>
+  <si>
+    <t>experimenter</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>does the subject concent entering to a lab-db (no contact details)</t>
+  </si>
+  <si>
+    <t>does the subject concents to enter contact details to db to be contacted again</t>
+  </si>
+  <si>
+    <t>phone/email/no</t>
+  </si>
+  <si>
+    <t>Does he answer all Criteria?</t>
+  </si>
+  <si>
+    <t>Khen heller</t>
+  </si>
+  <si>
+    <t>118B</t>
+  </si>
+  <si>
+    <t>Using 6 cameras</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Hebrew</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>payment</t>
+  </si>
+  <si>
+    <t>16.2.21</t>
+  </si>
+  <si>
+    <t>Running on myself to check if masks timings faulty in trials 72 and 38 still occurs</t>
+  </si>
+  <si>
+    <t>Running on myself to check if masks timings faulty in trials 72 and 38 still occurs. In trials 80 and on I put my finger to the screen before target was displayed</t>
+  </si>
+  <si>
+    <t>Ran on myself, to check why categor time is NaN when I touch screen before target is displayed</t>
+  </si>
+  <si>
+    <t>Same as up, but used trials4.xlsx to compare to 1001</t>
+  </si>
+  <si>
+    <t>This time disconnected internet and put high priority</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +213,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +535,848 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AI19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V16" sqref="V16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="12.625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+    </row>
+    <row r="2" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="4">
+        <v>1</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="4">
+        <v>1</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="4">
+        <v>1</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="4">
+        <v>1</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="4">
+        <v>1</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="4">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="4">
+        <v>1</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="4">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="4">
+        <v>1</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="4">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O10" s="4">
+        <v>1</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="4">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O11" s="4">
+        <v>1</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="4">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12" s="4">
+        <v>1</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1001</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" s="4">
+        <v>1</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1002</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" s="4">
+        <v>1</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1003</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" s="4">
+        <v>1</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1005</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" s="4">
+        <v>1</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="V16" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1004</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O19" s="4">
+        <v>1</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U19" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add screen alignment func
</commit_message>
<xml_diff>
--- a/experiment/subject_log.xlsx
+++ b/experiment/subject_log.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\khen_heller\subliminal_priming_w_motion_capture\experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D9E0DA-A09E-4626-AC18-68B5B4DA8CFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="51">
   <si>
     <t>date</t>
   </si>
@@ -152,9 +153,6 @@
     <t>11.3.21</t>
   </si>
   <si>
-    <t>Full run on myself to check timing</t>
-  </si>
-  <si>
     <t>14.3.21</t>
   </si>
   <si>
@@ -171,12 +169,21 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>24.3.21</t>
+  </si>
+  <si>
+    <t>Full run on myself with full arm reach to check analysis code and see if b-spline fits data well</t>
+  </si>
+  <si>
+    <t>Full run on myself with short reach distance (only finger movement) to check timing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -259,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -280,6 +287,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -561,17 +571,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.875" style="4" bestFit="1" customWidth="1"/>
@@ -696,7 +706,7 @@
     </row>
     <row r="3" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -711,16 +721,16 @@
         <v>31</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>32</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>40</v>
@@ -1443,12 +1453,12 @@
         <v>25</v>
       </c>
       <c r="U20" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="4">
         <v>1008</v>
@@ -1460,7 +1470,24 @@
         <v>25</v>
       </c>
       <c r="U21" s="4" t="s">
-        <v>42</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1009</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debug screen alignment func
</commit_message>
<xml_diff>
--- a/experiment/subject_log.xlsx
+++ b/experiment/subject_log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D9E0DA-A09E-4626-AC18-68B5B4DA8CFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD90273-CD01-4ABA-A4E8-16027A90D1B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="56">
   <si>
     <t>date</t>
   </si>
@@ -178,6 +178,21 @@
   </si>
   <si>
     <t>Full run on myself with short reach distance (only finger movement) to check timing</t>
+  </si>
+  <si>
+    <t>11.4.21</t>
+  </si>
+  <si>
+    <t>Full run on myself with full arm reach to check to make sure all ok before running subs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full run on myself with full arm reach to check timing on diff screen (Asus, refrate 100) </t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>12.4.21</t>
   </si>
 </sst>
 </file>
@@ -572,11 +587,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI22"/>
+  <dimension ref="A1:AI24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U21" sqref="U21"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -770,20 +785,47 @@
       </c>
     </row>
     <row r="4" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="B4" s="4">
         <v>2</v>
       </c>
+      <c r="C4" s="4">
+        <v>30</v>
+      </c>
       <c r="D4" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="H4" s="4" t="s">
         <v>32</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>33</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="O4" s="4">
         <v>1</v>
@@ -1488,6 +1530,40 @@
       </c>
       <c r="U22" s="4" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="4">
+        <v>1010</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1011</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U24" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add RT and traj STD analysis
</commit_message>
<xml_diff>
--- a/experiment/subject_log.xlsx
+++ b/experiment/subject_log.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\khen_heller\subliminal_priming_w_motion_capture\experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD90273-CD01-4ABA-A4E8-16027A90D1B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="59">
   <si>
     <t>date</t>
   </si>
@@ -193,13 +192,22 @@
   </si>
   <si>
     <t>12.4.21</t>
+  </si>
+  <si>
+    <t>13.4.21</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>netayellin97@walla.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +237,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -278,10 +294,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -307,8 +324,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -586,12 +607,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -850,20 +871,47 @@
       </c>
     </row>
     <row r="5" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="B5" s="4">
         <v>3</v>
       </c>
+      <c r="C5" s="4">
+        <v>24</v>
+      </c>
       <c r="D5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="H5" s="4" t="s">
         <v>32</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>33</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="O5" s="4">
         <v>1</v>
@@ -1567,7 +1615,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added runTests that runs tests on subs
</commit_message>
<xml_diff>
--- a/experiment/subject_log.xlsx
+++ b/experiment/subject_log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="71">
   <si>
     <t>date</t>
   </si>
@@ -207,6 +207,36 @@
   </si>
   <si>
     <t>ela4610@gmail.com</t>
+  </si>
+  <si>
+    <t>21.4.21</t>
+  </si>
+  <si>
+    <t>lenses</t>
+  </si>
+  <si>
+    <t>naomivaknine@mail.tau.ac.il</t>
+  </si>
+  <si>
+    <t>peleg4008@gmail.com</t>
+  </si>
+  <si>
+    <t>26.4.21</t>
+  </si>
+  <si>
+    <t>credit</t>
+  </si>
+  <si>
+    <t>tamarsela@mail.tau.ac.il</t>
+  </si>
+  <si>
+    <t>rotemasher98@gmail.com</t>
+  </si>
+  <si>
+    <t>27.4.21</t>
+  </si>
+  <si>
+    <t>yuvalheimann@mail.tau.ac.il</t>
   </si>
 </sst>
 </file>
@@ -614,11 +644,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI24"/>
+  <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T6" sqref="T6"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1007,21 +1037,48 @@
       </c>
     </row>
     <row r="7" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B7" s="4">
         <v>5</v>
       </c>
+      <c r="C7" s="4">
+        <v>24</v>
+      </c>
       <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="H7" s="4" t="s">
         <v>32</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="L7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="O7" s="4">
         <v>1</v>
       </c>
@@ -1045,21 +1102,48 @@
       </c>
     </row>
     <row r="8" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B8" s="4">
         <v>6</v>
       </c>
+      <c r="C8" s="4">
+        <v>22</v>
+      </c>
       <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="H8" s="4" t="s">
         <v>32</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="L8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="O8" s="4">
         <v>1</v>
       </c>
@@ -1083,20 +1167,47 @@
       </c>
     </row>
     <row r="9" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="B9" s="4">
         <v>7</v>
       </c>
+      <c r="C9" s="4">
+        <v>23</v>
+      </c>
       <c r="D9" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="H9" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="I9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="K9" s="4" t="s">
-        <v>33</v>
+        <v>66</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="O9" s="4">
         <v>1</v>
@@ -1121,20 +1232,47 @@
       </c>
     </row>
     <row r="10" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="B10" s="4">
         <v>8</v>
       </c>
+      <c r="C10" s="4">
+        <v>22</v>
+      </c>
       <c r="D10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="H10" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="I10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="K10" s="4" t="s">
-        <v>33</v>
+        <v>66</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="O10" s="4">
         <v>1</v>
@@ -1159,20 +1297,47 @@
       </c>
     </row>
     <row r="11" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="B11" s="4">
         <v>9</v>
       </c>
+      <c r="C11" s="4">
+        <v>25</v>
+      </c>
       <c r="D11" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="F11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="H11" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="I11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="K11" s="4" t="s">
-        <v>33</v>
+        <v>66</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="O11" s="4">
         <v>1</v>
@@ -1197,21 +1362,13 @@
       </c>
     </row>
     <row r="12" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="B12" s="4">
         <v>10</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="N12" s="9"/>
       <c r="O12" s="4">
         <v>1</v>
       </c>
@@ -1644,6 +1801,20 @@
         <v>25</v>
       </c>
       <c r="U24" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1012</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U25" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1651,8 +1822,13 @@
   <hyperlinks>
     <hyperlink ref="N5" r:id="rId1"/>
     <hyperlink ref="N6" r:id="rId2"/>
+    <hyperlink ref="N7" r:id="rId3"/>
+    <hyperlink ref="N8" r:id="rId4"/>
+    <hyperlink ref="N9" r:id="rId5"/>
+    <hyperlink ref="N10" r:id="rId6"/>
+    <hyperlink ref="N11" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add option to analyze only 1 traj | Add PAS | RT, Traj, Pas on same figure
Add std to beeswarm
</commit_message>
<xml_diff>
--- a/experiment/subject_log.xlsx
+++ b/experiment/subject_log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="72">
   <si>
     <t>date</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>yuvalheimann@mail.tau.ac.il</t>
+  </si>
+  <si>
+    <t>2.5.21</t>
   </si>
 </sst>
 </file>
@@ -646,9 +649,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1363,10 +1366,40 @@
     </row>
     <row r="12" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B12" s="4">
         <v>10</v>
+      </c>
+      <c r="C12" s="4">
+        <v>23</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="N12" s="9"/>
       <c r="O12" s="4">

</xml_diff>

<commit_message>
debug practice w/o prime
</commit_message>
<xml_diff>
--- a/experiment/subject_log.xlsx
+++ b/experiment/subject_log.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\khen_heller\subliminal_priming_w_motion_capture\experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1886FD94-CA94-4682-98EC-05F5E46621EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="83">
   <si>
     <t>date</t>
   </si>
@@ -252,12 +253,33 @@
   </si>
   <si>
     <t>26.5.21</t>
+  </si>
+  <si>
+    <t>27.5.21</t>
+  </si>
+  <si>
+    <t>Full run on myself with full arm reach, Changed "no prime train" trial list.</t>
+  </si>
+  <si>
+    <t>2, add "no prime training", split RT and shorten it to 750.</t>
+  </si>
+  <si>
+    <t>Arabic</t>
+  </si>
+  <si>
+    <t>talsasson1@mail.tau.ac.il</t>
+  </si>
+  <si>
+    <t>Reach dist 35cm</t>
+  </si>
+  <si>
+    <t>Reach dist 40cm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -658,12 +680,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AI47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomLeft" activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -853,7 +875,7 @@
         <v>25</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -918,7 +940,7 @@
         <v>25</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -983,7 +1005,7 @@
         <v>25</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1048,7 +1070,7 @@
         <v>25</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1113,7 +1135,7 @@
         <v>25</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1178,7 +1200,7 @@
         <v>25</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1243,7 +1265,7 @@
         <v>25</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1308,7 +1330,7 @@
         <v>25</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1373,7 +1395,7 @@
         <v>25</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1433,54 +1455,54 @@
         <v>25</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B13" s="4">
-        <v>1001</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>28</v>
+        <v>11</v>
+      </c>
+      <c r="C13" s="4">
+        <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O13" s="4">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="P13" s="4" t="s">
         <v>26</v>
@@ -1498,54 +1520,54 @@
         <v>25</v>
       </c>
       <c r="U13" s="4" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="B14" s="4">
-        <v>1002</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="C14" s="4">
+        <v>26</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O14" s="4">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="P14" s="4" t="s">
         <v>26</v>
@@ -1563,54 +1585,24 @@
         <v>25</v>
       </c>
       <c r="U14" s="4" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B15" s="4">
-        <v>1003</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O15" s="4">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="P15" s="4" t="s">
         <v>26</v>
@@ -1628,330 +1620,765 @@
         <v>25</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="4">
+        <v>14</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="4">
+        <v>15</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U17" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="4">
+        <v>16</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U18" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="4">
+        <v>17</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U19" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="4">
+        <v>18</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U20" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="4">
+        <v>19</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="4">
+        <v>20</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B23" s="4">
+        <v>1001</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O23" s="4">
+        <v>1</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1002</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" s="4">
+        <v>1</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U24" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1003</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O25" s="4">
+        <v>1</v>
+      </c>
+      <c r="P25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U25" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="4">
         <v>1005</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O16" s="4">
+      <c r="C26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O26" s="4">
         <v>1</v>
       </c>
-      <c r="P16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U16" s="6" t="s">
+      <c r="P26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U26" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="V16" s="7" t="s">
+      <c r="V26" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B29" s="4">
         <v>1004</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O19" s="4">
+      <c r="C29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O29" s="4">
         <v>1</v>
       </c>
-      <c r="P19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U19" s="4" t="s">
+      <c r="P29" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U29" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+    <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B30" s="4">
         <v>1007</v>
       </c>
-      <c r="P20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="T20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U20" s="4" t="s">
+      <c r="P30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U30" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B31" s="4">
         <v>1008</v>
       </c>
-      <c r="P21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="T21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U21" s="4" t="s">
+      <c r="P31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U31" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
+    <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B32" s="4">
         <v>1009</v>
       </c>
-      <c r="P22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="T22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U22" s="4" t="s">
+      <c r="P32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U32" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="33" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B33" s="4">
         <v>1010</v>
       </c>
-      <c r="P23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="T23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U23" s="4" t="s">
+      <c r="P33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U33" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+    <row r="34" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B34" s="4">
         <v>1011</v>
       </c>
-      <c r="P24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="T24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U24" s="4" t="s">
+      <c r="P34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T34" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U34" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+    <row r="35" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B35" s="4">
         <v>1012</v>
       </c>
-      <c r="T25" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U25" s="4" t="s">
+      <c r="T35" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U35" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+    <row r="36" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B36" s="4">
         <v>1013</v>
       </c>
-      <c r="T26" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U26" s="4" t="s">
+      <c r="T36" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U36" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+    <row r="37" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B37" s="4">
         <v>1014</v>
       </c>
-      <c r="T27" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U27" s="4" t="s">
+      <c r="T37" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U37" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T28" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T29" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T30" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T31" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T32" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="20:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T33" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="20:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T34" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="20:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T35" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="20:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T36" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="20:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T37" s="4" t="s">
+    <row r="38" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1015</v>
+      </c>
+      <c r="T38" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U38" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T39" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T40" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T41" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T42" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T43" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T44" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T45" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T46" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T47" s="4" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N5" r:id="rId1"/>
-    <hyperlink ref="N6" r:id="rId2"/>
-    <hyperlink ref="N7" r:id="rId3"/>
-    <hyperlink ref="N8" r:id="rId4"/>
-    <hyperlink ref="N9" r:id="rId5"/>
-    <hyperlink ref="N10" r:id="rId6"/>
-    <hyperlink ref="N11" r:id="rId7"/>
+    <hyperlink ref="N5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="N6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="N7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="N8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="N9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="N10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="N11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="N14" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed vars called 'type'
</commit_message>
<xml_diff>
--- a/experiment/subject_log.xlsx
+++ b/experiment/subject_log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="87">
   <si>
     <t>date</t>
   </si>
@@ -267,6 +267,24 @@
   </si>
   <si>
     <t>talsasson1@mail.tau.ac.il</t>
+  </si>
+  <si>
+    <t>1.7.21</t>
+  </si>
+  <si>
+    <t>Don’t know what I did here</t>
+  </si>
+  <si>
+    <t>Full run on myself with full arm reach, Recording in Optitrack during experiment</t>
+  </si>
+  <si>
+    <t>4.7.21</t>
+  </si>
+  <si>
+    <t>Full run on myself with full arm reach, Recording in Optitrack during experiment, Passive recording</t>
+  </si>
+  <si>
+    <t>5.7.21</t>
   </si>
 </sst>
 </file>
@@ -676,9 +694,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U42" sqref="U42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2370,23 +2388,59 @@
       </c>
     </row>
     <row r="39" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1016</v>
+      </c>
       <c r="T39" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="U39" s="4" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="4">
+        <v>1017</v>
+      </c>
       <c r="T40" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="U40" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="41" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1018</v>
+      </c>
       <c r="T41" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="U41" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="42" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" s="4">
+        <v>1019</v>
+      </c>
       <c r="T42" s="4" t="s">
         <v>25</v>
+      </c>
+      <c r="U42" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixed dates in sub_log
</commit_message>
<xml_diff>
--- a/experiment/subject_log.xlsx
+++ b/experiment/subject_log.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\khen_heller\subliminal_priming_w_motion_capture\experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603273A5-70DA-4FC4-AB73-50ED9B805CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="87">
   <si>
     <t>date</t>
   </si>
@@ -197,45 +198,24 @@
     <t>left</t>
   </si>
   <si>
-    <t>netayellin97@walla.com</t>
-  </si>
-  <si>
     <t>18.4.21</t>
   </si>
   <si>
-    <t>ela4610@gmail.com</t>
-  </si>
-  <si>
     <t>21.4.21</t>
   </si>
   <si>
     <t>lenses</t>
   </si>
   <si>
-    <t>naomivaknine@mail.tau.ac.il</t>
-  </si>
-  <si>
-    <t>peleg4008@gmail.com</t>
-  </si>
-  <si>
     <t>26.4.21</t>
   </si>
   <si>
     <t>credit</t>
   </si>
   <si>
-    <t>tamarsela@mail.tau.ac.il</t>
-  </si>
-  <si>
-    <t>rotemasher98@gmail.com</t>
-  </si>
-  <si>
     <t>27.4.21</t>
   </si>
   <si>
-    <t>yuvalheimann@mail.tau.ac.il</t>
-  </si>
-  <si>
     <t>2.5.21</t>
   </si>
   <si>
@@ -263,9 +243,6 @@
     <t>Arabic</t>
   </si>
   <si>
-    <t>talsasson1@mail.tau.ac.il</t>
-  </si>
-  <si>
     <t>1.7.21</t>
   </si>
   <si>
@@ -303,12 +280,18 @@
   </si>
   <si>
     <t>Full run on myself with full arm reach, recording traj from fixation, recognize screen touch only after target display.</t>
+  </si>
+  <si>
+    <t>31.5.21</t>
+  </si>
+  <si>
+    <t>3.6.21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -709,12 +692,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AI58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U45" sqref="U45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -809,7 +792,7 @@
         <v>20</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
@@ -1015,9 +998,7 @@
       <c r="M5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="9" t="s">
-        <v>57</v>
-      </c>
+      <c r="N5" s="9"/>
       <c r="O5" s="4">
         <v>1</v>
       </c>
@@ -1042,7 +1023,7 @@
     </row>
     <row r="6" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4">
         <v>4</v>
@@ -1080,9 +1061,7 @@
       <c r="M6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="9" t="s">
-        <v>59</v>
-      </c>
+      <c r="N6" s="9"/>
       <c r="O6" s="4">
         <v>1</v>
       </c>
@@ -1107,7 +1086,7 @@
     </row>
     <row r="7" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" s="4">
         <v>5</v>
@@ -1125,7 +1104,7 @@
         <v>56</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>32</v>
@@ -1145,9 +1124,7 @@
       <c r="M7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="N7" s="9"/>
       <c r="O7" s="4">
         <v>1</v>
       </c>
@@ -1172,7 +1149,7 @@
     </row>
     <row r="8" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B8" s="4">
         <v>6</v>
@@ -1210,9 +1187,7 @@
       <c r="M8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N8" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="N8" s="9"/>
       <c r="O8" s="4">
         <v>1</v>
       </c>
@@ -1237,7 +1212,7 @@
     </row>
     <row r="9" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B9" s="4">
         <v>7</v>
@@ -1255,7 +1230,7 @@
         <v>44</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>32</v>
@@ -1267,7 +1242,7 @@
         <v>39</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>39</v>
@@ -1275,9 +1250,7 @@
       <c r="M9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="N9" s="9"/>
       <c r="O9" s="4">
         <v>1</v>
       </c>
@@ -1302,7 +1275,7 @@
     </row>
     <row r="10" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B10" s="4">
         <v>8</v>
@@ -1332,7 +1305,7 @@
         <v>39</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>39</v>
@@ -1340,9 +1313,7 @@
       <c r="M10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N10" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="N10" s="9"/>
       <c r="O10" s="4">
         <v>1</v>
       </c>
@@ -1367,7 +1338,7 @@
     </row>
     <row r="11" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B11" s="4">
         <v>9</v>
@@ -1397,7 +1368,7 @@
         <v>39</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>39</v>
@@ -1405,9 +1376,7 @@
       <c r="M11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N11" s="9" t="s">
-        <v>69</v>
-      </c>
+      <c r="N11" s="9"/>
       <c r="O11" s="4">
         <v>1</v>
       </c>
@@ -1432,7 +1401,7 @@
     </row>
     <row r="12" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B12" s="4">
         <v>10</v>
@@ -1462,7 +1431,7 @@
         <v>39</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>32</v>
@@ -1492,7 +1461,7 @@
     </row>
     <row r="13" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B13" s="4">
         <v>11</v>
@@ -1501,7 +1470,7 @@
         <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>31</v>
@@ -1522,7 +1491,7 @@
         <v>39</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>32</v>
@@ -1530,11 +1499,8 @@
       <c r="M13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N13" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="O13" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="P13" s="4" t="s">
         <v>26</v>
@@ -1557,7 +1523,7 @@
     </row>
     <row r="14" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B14" s="4">
         <v>12</v>
@@ -1575,7 +1541,7 @@
         <v>44</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>32</v>
@@ -1587,7 +1553,7 @@
         <v>39</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>39</v>
@@ -1595,11 +1561,9 @@
       <c r="M14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N14" s="9" t="s">
-        <v>79</v>
-      </c>
+      <c r="N14" s="9"/>
       <c r="O14" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="P14" s="4" t="s">
         <v>26</v>
@@ -1622,7 +1586,7 @@
     </row>
     <row r="15" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="B15" s="4">
         <v>13</v>
@@ -1640,7 +1604,7 @@
         <v>44</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>32</v>
@@ -1652,7 +1616,7 @@
         <v>32</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>32</v>
@@ -1661,7 +1625,7 @@
         <v>29</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="P15" s="4" t="s">
         <v>26</v>
@@ -1684,7 +1648,7 @@
     </row>
     <row r="16" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="B16" s="4">
         <v>14</v>
@@ -1714,7 +1678,7 @@
         <v>32</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>32</v>
@@ -1723,7 +1687,7 @@
         <v>29</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="P16" s="4" t="s">
         <v>26</v>
@@ -1744,21 +1708,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>60</v>
-      </c>
+    <row r="17" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="4">
         <v>15</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="P17" s="4" t="s">
         <v>26</v>
@@ -1779,21 +1740,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>60</v>
-      </c>
+    <row r="18" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4">
         <v>16</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="P18" s="4" t="s">
         <v>26</v>
@@ -1814,21 +1772,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>64</v>
-      </c>
+    <row r="19" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="4">
         <v>17</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="P19" s="4" t="s">
         <v>26</v>
@@ -1849,21 +1804,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>64</v>
-      </c>
+    <row r="20" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="4">
         <v>18</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="P20" s="4" t="s">
         <v>26</v>
@@ -1884,21 +1836,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>68</v>
-      </c>
+    <row r="21" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="4">
         <v>19</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="P21" s="4" t="s">
         <v>26</v>
@@ -1919,21 +1868,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>70</v>
-      </c>
+    <row r="22" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="4">
         <v>20</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="P22" s="4" t="s">
         <v>26</v>
@@ -1957,656 +1903,646 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B34" s="4">
         <v>1001</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O23" s="4">
+      <c r="C34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O34" s="4">
         <v>1</v>
       </c>
-      <c r="P23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U23" s="4" t="s">
+      <c r="P34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T34" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="V23" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="V34" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B35" s="4">
         <v>1002</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O24" s="4">
+      <c r="C35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O35" s="4">
         <v>1</v>
       </c>
-      <c r="P24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U24" s="4" t="s">
+      <c r="P35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T35" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U35" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="V24" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="V35" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B36" s="4">
         <v>1003</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O25" s="4">
+      <c r="C36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O36" s="4">
         <v>1</v>
       </c>
-      <c r="P25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T25" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U25" s="4" t="s">
+      <c r="P36" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T36" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U36" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="V25" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="V36" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B37" s="4">
         <v>1005</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O26" s="4">
+      <c r="C37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O37" s="4">
         <v>1</v>
       </c>
-      <c r="P26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T26" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U26" s="6" t="s">
+      <c r="P37" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T37" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U37" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="V26" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V27" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V28" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="V37" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V38" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V39" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B40" s="4">
         <v>1004</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O29" s="4">
+      <c r="C40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O40" s="4">
         <v>1</v>
       </c>
-      <c r="P29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T29" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U29" s="4" t="s">
+      <c r="P40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T40" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U40" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="V29" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="V40" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B41" s="4">
         <v>1007</v>
       </c>
-      <c r="P30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="T30" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U30" s="4" t="s">
+      <c r="P41" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T41" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U41" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="V30" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="V41" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B42" s="4">
         <v>1008</v>
       </c>
-      <c r="P31" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="T31" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U31" s="4" t="s">
+      <c r="P42" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T42" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U42" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="V31" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
+      <c r="V42" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B43" s="4">
         <v>1009</v>
       </c>
-      <c r="P32" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="T32" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U32" s="4" t="s">
+      <c r="P43" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T43" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U43" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="V32" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="V43" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B44" s="4">
         <v>1010</v>
       </c>
-      <c r="P33" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="T33" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U33" s="4" t="s">
+      <c r="P44" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T44" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U44" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="V33" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="V44" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B45" s="4">
         <v>1011</v>
       </c>
-      <c r="P34" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="T34" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U34" s="4" t="s">
+      <c r="P45" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T45" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U45" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="V34" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="V45" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="4">
+        <v>1012</v>
+      </c>
+      <c r="T46" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U46" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="V46" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="4">
+        <v>1013</v>
+      </c>
+      <c r="T47" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U47" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="V47" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1014</v>
+      </c>
+      <c r="T48" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U48" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="V48" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="4">
-        <v>1012</v>
-      </c>
-      <c r="T35" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U35" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="V35" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="4">
-        <v>1013</v>
-      </c>
-      <c r="T36" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U36" s="4" t="s">
+      <c r="B49" s="4">
+        <v>1015</v>
+      </c>
+      <c r="T49" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U49" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="V49" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="4">
+        <v>1016</v>
+      </c>
+      <c r="T50" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U50" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="V50" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V36" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="B51" s="4">
+        <v>1017</v>
+      </c>
+      <c r="T51" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U51" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="4">
-        <v>1014</v>
-      </c>
-      <c r="T37" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U37" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="V37" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+      <c r="V51" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="4">
-        <v>1015</v>
-      </c>
-      <c r="T38" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U38" s="4" t="s">
+      <c r="B52" s="4">
+        <v>1018</v>
+      </c>
+      <c r="T52" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U52" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="V38" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="4">
-        <v>1016</v>
-      </c>
-      <c r="T39" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U39" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="V39" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+      <c r="V52" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="4">
+        <v>1019</v>
+      </c>
+      <c r="T53" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U53" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="V53" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="4">
+        <v>1020</v>
+      </c>
+      <c r="T54" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U54" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="V54" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B40" s="4">
-        <v>1017</v>
-      </c>
-      <c r="T40" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U40" s="4" t="s">
+      <c r="W54" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="V40" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+      <c r="B55" s="4">
+        <v>1021</v>
+      </c>
+      <c r="T55" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U55" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="V55" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="4">
-        <v>1018</v>
-      </c>
-      <c r="T41" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U41" s="4" t="s">
+      <c r="W55" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" s="4">
+        <v>1022</v>
+      </c>
+      <c r="T56" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U56" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="V41" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="4">
-        <v>1019</v>
-      </c>
-      <c r="T42" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U42" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="V42" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B43" s="4">
-        <v>1020</v>
-      </c>
-      <c r="T43" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U43" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="V43" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="W43" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B44" s="4">
-        <v>1021</v>
-      </c>
-      <c r="T44" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U44" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="V44" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="W44" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" s="4">
-        <v>1022</v>
-      </c>
-      <c r="T45" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U45" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="W45" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T46" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T47" s="4" t="s">
+      <c r="W56" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T57" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T58" s="4" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="N5" r:id="rId1"/>
-    <hyperlink ref="N6" r:id="rId2"/>
-    <hyperlink ref="N7" r:id="rId3"/>
-    <hyperlink ref="N8" r:id="rId4"/>
-    <hyperlink ref="N9" r:id="rId5"/>
-    <hyperlink ref="N10" r:id="rId6"/>
-    <hyperlink ref="N11" r:id="rId7"/>
-    <hyperlink ref="N14" r:id="rId8"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "fixed dates in sub_log"
This reverts commit 53c95fa3edc06636c29a75beae7da1e36262a663.
</commit_message>
<xml_diff>
--- a/experiment/subject_log.xlsx
+++ b/experiment/subject_log.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\khen_heller\subliminal_priming_w_motion_capture\experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603273A5-70DA-4FC4-AB73-50ED9B805CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="93">
   <si>
     <t>date</t>
   </si>
@@ -198,24 +197,45 @@
     <t>left</t>
   </si>
   <si>
+    <t>netayellin97@walla.com</t>
+  </si>
+  <si>
     <t>18.4.21</t>
   </si>
   <si>
+    <t>ela4610@gmail.com</t>
+  </si>
+  <si>
     <t>21.4.21</t>
   </si>
   <si>
     <t>lenses</t>
   </si>
   <si>
+    <t>naomivaknine@mail.tau.ac.il</t>
+  </si>
+  <si>
+    <t>peleg4008@gmail.com</t>
+  </si>
+  <si>
     <t>26.4.21</t>
   </si>
   <si>
     <t>credit</t>
   </si>
   <si>
+    <t>tamarsela@mail.tau.ac.il</t>
+  </si>
+  <si>
+    <t>rotemasher98@gmail.com</t>
+  </si>
+  <si>
     <t>27.4.21</t>
   </si>
   <si>
+    <t>yuvalheimann@mail.tau.ac.il</t>
+  </si>
+  <si>
     <t>2.5.21</t>
   </si>
   <si>
@@ -243,6 +263,9 @@
     <t>Arabic</t>
   </si>
   <si>
+    <t>talsasson1@mail.tau.ac.il</t>
+  </si>
+  <si>
     <t>1.7.21</t>
   </si>
   <si>
@@ -280,18 +303,12 @@
   </si>
   <si>
     <t>Full run on myself with full arm reach, recording traj from fixation, recognize screen touch only after target display.</t>
-  </si>
-  <si>
-    <t>31.5.21</t>
-  </si>
-  <si>
-    <t>3.6.21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -692,12 +709,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -792,7 +809,7 @@
         <v>20</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
@@ -998,7 +1015,9 @@
       <c r="M5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="9"/>
+      <c r="N5" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="O5" s="4">
         <v>1</v>
       </c>
@@ -1023,7 +1042,7 @@
     </row>
     <row r="6" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B6" s="4">
         <v>4</v>
@@ -1061,7 +1080,9 @@
       <c r="M6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="9"/>
+      <c r="N6" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="O6" s="4">
         <v>1</v>
       </c>
@@ -1086,7 +1107,7 @@
     </row>
     <row r="7" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B7" s="4">
         <v>5</v>
@@ -1104,7 +1125,7 @@
         <v>56</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>32</v>
@@ -1124,7 +1145,9 @@
       <c r="M7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="9"/>
+      <c r="N7" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="O7" s="4">
         <v>1</v>
       </c>
@@ -1149,7 +1172,7 @@
     </row>
     <row r="8" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B8" s="4">
         <v>6</v>
@@ -1187,7 +1210,9 @@
       <c r="M8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N8" s="9"/>
+      <c r="N8" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="O8" s="4">
         <v>1</v>
       </c>
@@ -1212,7 +1237,7 @@
     </row>
     <row r="9" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B9" s="4">
         <v>7</v>
@@ -1230,7 +1255,7 @@
         <v>44</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>32</v>
@@ -1242,7 +1267,7 @@
         <v>39</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>39</v>
@@ -1250,7 +1275,9 @@
       <c r="M9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="9"/>
+      <c r="N9" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="O9" s="4">
         <v>1</v>
       </c>
@@ -1275,7 +1302,7 @@
     </row>
     <row r="10" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B10" s="4">
         <v>8</v>
@@ -1305,7 +1332,7 @@
         <v>39</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>39</v>
@@ -1313,7 +1340,9 @@
       <c r="M10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N10" s="9"/>
+      <c r="N10" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="O10" s="4">
         <v>1</v>
       </c>
@@ -1338,7 +1367,7 @@
     </row>
     <row r="11" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B11" s="4">
         <v>9</v>
@@ -1368,7 +1397,7 @@
         <v>39</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>39</v>
@@ -1376,7 +1405,9 @@
       <c r="M11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N11" s="9"/>
+      <c r="N11" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="O11" s="4">
         <v>1</v>
       </c>
@@ -1401,7 +1432,7 @@
     </row>
     <row r="12" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B12" s="4">
         <v>10</v>
@@ -1431,7 +1462,7 @@
         <v>39</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>32</v>
@@ -1461,7 +1492,7 @@
     </row>
     <row r="13" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="B13" s="4">
         <v>11</v>
@@ -1470,7 +1501,7 @@
         <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>31</v>
@@ -1491,7 +1522,7 @@
         <v>39</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>32</v>
@@ -1499,8 +1530,11 @@
       <c r="M13" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="N13" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="O13" s="4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="P13" s="4" t="s">
         <v>26</v>
@@ -1523,7 +1557,7 @@
     </row>
     <row r="14" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B14" s="4">
         <v>12</v>
@@ -1541,7 +1575,7 @@
         <v>44</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>32</v>
@@ -1553,7 +1587,7 @@
         <v>39</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>39</v>
@@ -1561,9 +1595,11 @@
       <c r="M14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N14" s="9"/>
+      <c r="N14" s="9" t="s">
+        <v>79</v>
+      </c>
       <c r="O14" s="4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="P14" s="4" t="s">
         <v>26</v>
@@ -1586,7 +1622,7 @@
     </row>
     <row r="15" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B15" s="4">
         <v>13</v>
@@ -1604,7 +1640,7 @@
         <v>44</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>32</v>
@@ -1616,7 +1652,7 @@
         <v>32</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>32</v>
@@ -1625,7 +1661,7 @@
         <v>29</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="P15" s="4" t="s">
         <v>26</v>
@@ -1648,7 +1684,7 @@
     </row>
     <row r="16" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="B16" s="4">
         <v>14</v>
@@ -1678,7 +1714,7 @@
         <v>32</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>32</v>
@@ -1687,7 +1723,7 @@
         <v>29</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="P16" s="4" t="s">
         <v>26</v>
@@ -1708,18 +1744,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="B17" s="4">
         <v>15</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="P17" s="4" t="s">
         <v>26</v>
@@ -1740,18 +1779,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="B18" s="4">
         <v>16</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="P18" s="4" t="s">
         <v>26</v>
@@ -1772,18 +1814,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="B19" s="4">
         <v>17</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="P19" s="4" t="s">
         <v>26</v>
@@ -1804,18 +1849,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="B20" s="4">
         <v>18</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="P20" s="4" t="s">
         <v>26</v>
@@ -1836,18 +1884,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="B21" s="4">
         <v>19</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="P21" s="4" t="s">
         <v>26</v>
@@ -1868,18 +1919,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="B22" s="4">
         <v>20</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="P22" s="4" t="s">
         <v>26</v>
@@ -1903,646 +1957,656 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="4">
+        <v>1001</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O23" s="4">
+        <v>1</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1002</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" s="4">
+        <v>1</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="V24" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1003</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O25" s="4">
+        <v>1</v>
+      </c>
+      <c r="P25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="V25" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1005</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O26" s="4">
+        <v>1</v>
+      </c>
+      <c r="P26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U26" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="V26" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V27" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V28" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1004</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O29" s="4">
+        <v>1</v>
+      </c>
+      <c r="P29" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V29" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="4">
+        <v>1007</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U30" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="V30" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1008</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U31" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V31" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1009</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U32" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="V32" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="4">
+        <v>1010</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U33" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="V33" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B34" s="4">
-        <v>1001</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L34" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M34" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N34" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O34" s="4">
-        <v>1</v>
+        <v>1011</v>
       </c>
       <c r="P34" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="Q34" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R34" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S34" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="T34" s="4" t="s">
         <v>25</v>
       </c>
       <c r="U34" s="4" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="V34" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B35" s="4">
-        <v>1002</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L35" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M35" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N35" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O35" s="4">
-        <v>1</v>
-      </c>
-      <c r="P35" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q35" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R35" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S35" s="4" t="s">
-        <v>28</v>
+        <v>1012</v>
       </c>
       <c r="T35" s="4" t="s">
         <v>25</v>
       </c>
       <c r="U35" s="4" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="V35" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="B36" s="4">
-        <v>1003</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O36" s="4">
-        <v>1</v>
-      </c>
-      <c r="P36" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S36" s="4" t="s">
-        <v>28</v>
+        <v>1013</v>
       </c>
       <c r="T36" s="4" t="s">
         <v>25</v>
       </c>
       <c r="U36" s="4" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="V36" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="B37" s="4">
-        <v>1005</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O37" s="4">
-        <v>1</v>
-      </c>
-      <c r="P37" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S37" s="4" t="s">
-        <v>28</v>
+        <v>1014</v>
       </c>
       <c r="T37" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="U37" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="V37" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U37" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="V37" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1015</v>
+      </c>
+      <c r="T38" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U38" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="V38" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1016</v>
+      </c>
+      <c r="T39" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U39" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="V39" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="B40" s="4">
-        <v>1004</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O40" s="4">
-        <v>1</v>
-      </c>
-      <c r="P40" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S40" s="4" t="s">
-        <v>28</v>
+        <v>1017</v>
       </c>
       <c r="T40" s="4" t="s">
         <v>25</v>
       </c>
       <c r="U40" s="4" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="V40" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="B41" s="4">
-        <v>1007</v>
-      </c>
-      <c r="P41" s="4" t="s">
-        <v>26</v>
+        <v>1018</v>
       </c>
       <c r="T41" s="4" t="s">
         <v>25</v>
       </c>
       <c r="U41" s="4" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="V41" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="B42" s="4">
-        <v>1008</v>
-      </c>
-      <c r="P42" s="4" t="s">
-        <v>26</v>
+        <v>1019</v>
       </c>
       <c r="T42" s="4" t="s">
         <v>25</v>
       </c>
       <c r="U42" s="4" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="V42" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
-        <v>47</v>
+    <row r="43" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="B43" s="4">
-        <v>1009</v>
-      </c>
-      <c r="P43" s="4" t="s">
-        <v>26</v>
+        <v>1020</v>
       </c>
       <c r="T43" s="4" t="s">
         <v>25</v>
       </c>
       <c r="U43" s="4" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="V43" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="W43" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="B44" s="4">
-        <v>1010</v>
-      </c>
-      <c r="P44" s="4" t="s">
-        <v>26</v>
+        <v>1021</v>
       </c>
       <c r="T44" s="4" t="s">
         <v>25</v>
       </c>
       <c r="U44" s="4" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="V44" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+      <c r="W44" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="B45" s="4">
-        <v>1011</v>
-      </c>
-      <c r="P45" s="4" t="s">
-        <v>26</v>
+        <v>1022</v>
       </c>
       <c r="T45" s="4" t="s">
         <v>25</v>
       </c>
       <c r="U45" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="V45" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" s="4">
-        <v>1012</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="W45" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T46" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="U46" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="V46" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B47" s="4">
-        <v>1013</v>
-      </c>
+    </row>
+    <row r="47" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T47" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="U47" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="V47" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B48" s="4">
-        <v>1014</v>
-      </c>
-      <c r="T48" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U48" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="V48" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B49" s="4">
-        <v>1015</v>
-      </c>
-      <c r="T49" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U49" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="V49" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B50" s="4">
-        <v>1016</v>
-      </c>
-      <c r="T50" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U50" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="V50" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="51" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B51" s="4">
-        <v>1017</v>
-      </c>
-      <c r="T51" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U51" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="V51" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="52" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B52" s="4">
-        <v>1018</v>
-      </c>
-      <c r="T52" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U52" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="V52" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B53" s="4">
-        <v>1019</v>
-      </c>
-      <c r="T53" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U53" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="V53" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="54" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B54" s="4">
-        <v>1020</v>
-      </c>
-      <c r="T54" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U54" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="V54" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="W54" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="55" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55" s="4">
-        <v>1021</v>
-      </c>
-      <c r="T55" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U55" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="V55" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="W55" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="56" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" s="4">
-        <v>1022</v>
-      </c>
-      <c r="T56" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U56" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="W56" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="57" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T57" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="58" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T58" s="4" t="s">
-        <v>25</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N5" r:id="rId1"/>
+    <hyperlink ref="N6" r:id="rId2"/>
+    <hyperlink ref="N7" r:id="rId3"/>
+    <hyperlink ref="N8" r:id="rId4"/>
+    <hyperlink ref="N9" r:id="rId5"/>
+    <hyperlink ref="N10" r:id="rId6"/>
+    <hyperlink ref="N11" r:id="rId7"/>
+    <hyperlink ref="N14" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Debug last change"
This reverts commit f0eaf1cccfc31fd197850424b8f5524487c8002c.
</commit_message>
<xml_diff>
--- a/experiment/subject_log.xlsx
+++ b/experiment/subject_log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="91">
   <si>
     <t>date</t>
   </si>
@@ -290,19 +290,13 @@
     <t>Full run on myself with full arm reach, recording traj from fixation</t>
   </si>
   <si>
+    <t>didn’t succeed to run</t>
+  </si>
+  <si>
     <t>1846 times out of a total of 315263</t>
   </si>
   <si>
     <t>Missed stimulus presentation time</t>
-  </si>
-  <si>
-    <t>25.7.21</t>
-  </si>
-  <si>
-    <t>9793 times out of a total of 314105</t>
-  </si>
-  <si>
-    <t>Full run on myself with full arm reach, recording traj from fixation, recognize screen touch only after target display.</t>
   </si>
 </sst>
 </file>
@@ -712,9 +706,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U45" sqref="U45"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -809,7 +803,7 @@
         <v>20</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
@@ -2535,6 +2529,9 @@
       <c r="B43" s="4">
         <v>1020</v>
       </c>
+      <c r="C43" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="T43" s="4" t="s">
         <v>25</v>
       </c>
@@ -2542,47 +2539,20 @@
         <v>87</v>
       </c>
       <c r="V43" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="W43" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B44" s="4">
-        <v>1021</v>
-      </c>
       <c r="T44" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="U44" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="V44" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="W44" s="4" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="45" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" s="4">
-        <v>1022</v>
-      </c>
       <c r="T45" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="U45" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="W45" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Revert "changed vars called 'type'"
This reverts commit 75c9f44d21f12c6d9be60617d9f9d03dcde4d603.
</commit_message>
<xml_diff>
--- a/experiment/subject_log.xlsx
+++ b/experiment/subject_log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="81">
   <si>
     <t>date</t>
   </si>
@@ -267,24 +267,6 @@
   </si>
   <si>
     <t>talsasson1@mail.tau.ac.il</t>
-  </si>
-  <si>
-    <t>1.7.21</t>
-  </si>
-  <si>
-    <t>Don’t know what I did here</t>
-  </si>
-  <si>
-    <t>Full run on myself with full arm reach, Recording in Optitrack during experiment</t>
-  </si>
-  <si>
-    <t>4.7.21</t>
-  </si>
-  <si>
-    <t>Full run on myself with full arm reach, Recording in Optitrack during experiment, Passive recording</t>
-  </si>
-  <si>
-    <t>5.7.21</t>
   </si>
 </sst>
 </file>
@@ -694,9 +676,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U42" sqref="U42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2388,59 +2370,23 @@
       </c>
     </row>
     <row r="39" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="4">
-        <v>1016</v>
-      </c>
       <c r="T39" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="U39" s="4" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="4">
-        <v>1017</v>
-      </c>
       <c r="T40" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="U40" s="4" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="41" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B41" s="4">
-        <v>1018</v>
-      </c>
       <c r="T41" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="U41" s="4" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="42" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B42" s="4">
-        <v>1019</v>
-      </c>
       <c r="T42" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="U42" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>